<commit_message>
Added to Readme file
</commit_message>
<xml_diff>
--- a/Resources/Data/Price_Data/Book1.xlsx
+++ b/Resources/Data/Price_Data/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grothjd/DS_bootcamp/Project_1_Coffee_Price_Predictors/Resources/Data/Price_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3366E12A-9757-7045-9203-65519D075CDA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA957A6-8389-394E-BF9C-E0D9F8EA56C6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16420" xr2:uid="{19380059-405A-134D-BEBC-A57BE5E72E23}"/>
   </bookViews>
@@ -494,31 +494,35 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" customWidth="1"/>
     <col min="7" max="7" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="1"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" ht="21">
+      <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="21">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>0</v>

</xml_diff>